<commit_message>
modified excelsheet for the modules
</commit_message>
<xml_diff>
--- a/src/test/resources/config/TestData.xlsx
+++ b/src/test/resources/config/TestData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bloss\src\DsAlgoProject\src\test\resources\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF02E18-A00C-447E-AF16-F0911780BA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C7763F-E8BA-4551-BD94-B28F63007EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35085" yWindow="4575" windowWidth="18000" windowHeight="9150" xr2:uid="{E27DA2F6-63DD-46D2-91DF-3AEDC91BE982}"/>
+    <workbookView xWindow="3690" yWindow="1575" windowWidth="18000" windowHeight="9150" activeTab="1" xr2:uid="{E27DA2F6-63DD-46D2-91DF-3AEDC91BE982}"/>
   </bookViews>
   <sheets>
     <sheet name="python DS" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="3" r:id="rId2"/>
     <sheet name="Register" sheetId="2" r:id="rId3"/>
+    <sheet name="LinkedList" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
   <si>
     <t>Code</t>
   </si>
@@ -75,6 +76,36 @@
   </si>
   <si>
     <t xml:space="preserve">   password1</t>
+  </si>
+  <si>
+    <t>expected Outcome</t>
+  </si>
+  <si>
+    <t>popuperror message containing Syntaxerror</t>
+  </si>
+  <si>
+    <t>the user is able to see the output in the console</t>
+  </si>
+  <si>
+    <t>expectedOutcome</t>
+  </si>
+  <si>
+    <t>SyntaxError: bad input on line 1</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>Please fill out this field.</t>
+  </si>
+  <si>
+    <t>Invalid Username and Password</t>
+  </si>
+  <si>
+    <t>You are logged in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          output</t>
   </si>
 </sst>
 </file>
@@ -444,30 +475,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F067D1-C2DF-4A2E-AEFC-58BDD5A420B6}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -477,67 +518,93 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F2C110-56C1-4334-B7CD-8BDADEF0BA72}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -658,4 +725,48 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53766B52-149E-4428-9338-A08469D4814F}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
moved excel to pages and removed expected outcome
</commit_message>
<xml_diff>
--- a/src/test/resources/config/TestData.xlsx
+++ b/src/test/resources/config/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bloss\src\DsAlgoProject\src\test\resources\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1332eb67554a452f/Documents/DsAlgoProjectNew/src/test/resources/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF02E18-A00C-447E-AF16-F0911780BA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{CAF02E18-A00C-447E-AF16-F0911780BA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39E240FC-28ED-4E39-B6BE-465E3DA1DDF4}"/>
   <bookViews>
-    <workbookView xWindow="35085" yWindow="4575" windowWidth="18000" windowHeight="9150" xr2:uid="{E27DA2F6-63DD-46D2-91DF-3AEDC91BE982}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{E27DA2F6-63DD-46D2-91DF-3AEDC91BE982}"/>
   </bookViews>
   <sheets>
     <sheet name="python DS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t>Code</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t xml:space="preserve">   password1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expected Outcome  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">popup error message containing SyntaxError </t>
+  </si>
+  <si>
+    <t>the user is able to see the output in the console</t>
   </si>
 </sst>
 </file>
@@ -444,30 +453,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F067D1-C2DF-4A2E-AEFC-58BDD5A420B6}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.15234375" customWidth="1"/>
+    <col min="2" max="2" width="39.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -483,14 +502,14 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.3828125" customWidth="1"/>
+    <col min="2" max="2" width="20.69140625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -498,17 +517,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -516,7 +535,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -524,7 +543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -532,7 +551,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -561,14 +580,14 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.69140625" customWidth="1"/>
+    <col min="2" max="2" width="17.69140625" customWidth="1"/>
+    <col min="3" max="3" width="21.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -579,12 +598,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>11</v>
@@ -593,7 +612,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -604,7 +623,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -615,7 +634,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -626,7 +645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -637,7 +656,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Completed array and graph
</commit_message>
<xml_diff>
--- a/src/test/resources/config/TestData.xlsx
+++ b/src/test/resources/config/TestData.xlsx
@@ -3,18 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{14087A6E-4AD7-4EAE-A4C4-67BCDF9757CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sruja\DsalgoLatestSrujana\DsAlgoProject\src\test\resources\config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A70CDB-4C8A-46F9-BF79-CD33320E141E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="2" xr2:uid="{E27DA2F6-63DD-46D2-91DF-3AEDC91BE982}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{E27DA2F6-63DD-46D2-91DF-3AEDC91BE982}"/>
   </bookViews>
   <sheets>
     <sheet name="python DS" sheetId="1" r:id="rId1"/>
-    <sheet name="Login" sheetId="3" r:id="rId2"/>
-    <sheet name="Register" sheetId="2" r:id="rId3"/>
-    <sheet name="LinkedList" sheetId="4" r:id="rId4"/>
+    <sheet name="python PQ" sheetId="6" r:id="rId2"/>
+    <sheet name="Login" sheetId="3" r:id="rId3"/>
+    <sheet name="Register" sheetId="2" r:id="rId4"/>
+    <sheet name="LinkedList" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N21"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
   <si>
     <t>Code</t>
   </si>
@@ -102,13 +107,83 @@
   </si>
   <si>
     <t>You are logged in</t>
+  </si>
+  <si>
+    <t>def search(input_list, num):
+if(num in input_list):
+print("Element Found")
+\b
+\b
+else:
+print("Not Found")
+\b
+\b
+\b
+\b
+search([12, 23, 45, 67, 6, 90] , 12)</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums) :
+count = 0
+result = 0
+for i in range(0, len(nums)):
+if (nums[i] == 0):
+count = 0
+\b
+\b
+else:
+count+= 1
+\b
+\b
+result = max(result, count)
+\b
+\b
+print(result)
+\b
+\b
+findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+c=0
+for i in nums:
+j=str(i)
+x=len(j)
+if x%2==0:
+c=c+1
+\b
+\b
+\b
+\b
+print c
+return c
+findNumbers([12,345,2,6,7896])</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+squares_list = []
+for i in range(0, len(nums)):
+square = nums[i] * nums[i];
+squares_list.append(square)
+\b
+\b
+sorted_squares_list = sorted(squares_list)
+print sorted_squares_list;
+return sorted_squares_list;
+sortedSquares([-7,-3,2,3,11])</t>
+  </si>
+  <si>
+    <t>Element Found</t>
+  </si>
+  <si>
+    <t>[4, 9, 9, 49, 121]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,16 +205,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -147,22 +239,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{1D9FCDF7-B9F2-49B5-85F6-B98EAF40FB45}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -178,9 +291,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -218,7 +331,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -324,7 +437,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -466,7 +579,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -477,7 +590,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -516,6 +629,85 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8672DF5-F492-4ABF-91E8-B65E3B665CBD}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="212.08984375" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F2C110-56C1-4334-B7CD-8BDADEF0BA72}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -531,82 +723,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>25</v>
       </c>
     </row>
@@ -623,11 +811,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F460C870-84C0-4A56-9F22-2803FB76778D}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
@@ -639,85 +827,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="4"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -733,12 +918,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95301C7-7BF9-412A-A319-BF9742C03B37}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
changed Feature line in Tree
</commit_message>
<xml_diff>
--- a/src/test/resources/config/TestData.xlsx
+++ b/src/test/resources/config/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{14087A6E-4AD7-4EAE-A4C4-67BCDF9757CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4D0B2C4A-5642-4CA2-8A9E-7220BD293656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="2" xr2:uid="{E27DA2F6-63DD-46D2-91DF-3AEDC91BE982}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="3" xr2:uid="{E27DA2F6-63DD-46D2-91DF-3AEDC91BE982}"/>
   </bookViews>
   <sheets>
     <sheet name="python DS" sheetId="1" r:id="rId1"/>
@@ -152,13 +152,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -531,82 +529,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>25</v>
       </c>
     </row>
@@ -627,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F460C870-84C0-4A56-9F22-2803FB76778D}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
@@ -639,85 +633,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="4"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -737,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95301C7-7BF9-412A-A319-BF9742C03B37}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -748,26 +740,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes fixed with url
</commit_message>
<xml_diff>
--- a/src/test/resources/config/TestData.xlsx
+++ b/src/test/resources/config/TestData.xlsx
@@ -3,14 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sruja\DsalgoLatestSrujana\DsAlgoProject\src\test\resources\config\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A12CF6C-5B40-48B7-B7C6-D6B185CF5B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9D8B890F-5F59-4A55-856A-EDA6FBA47775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="4" xr2:uid="{E27DA2F6-63DD-46D2-91DF-3AEDC91BE982}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{E27DA2F6-63DD-46D2-91DF-3AEDC91BE982}"/>
   </bookViews>
   <sheets>
     <sheet name="python DS" sheetId="1" r:id="rId1"/>
@@ -20,6 +15,7 @@
     <sheet name="LinkedList" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="B1:P13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -260,17 +256,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -291,9 +288,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -331,7 +328,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -437,7 +434,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -579,7 +576,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -632,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8672DF5-F492-4ABF-91E8-B65E3B665CBD}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -643,58 +640,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>31</v>
       </c>
     </row>
@@ -921,7 +918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95301C7-7BF9-412A-A319-BF9742C03B37}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
@@ -932,26 +929,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>